<commit_message>
Trying to get Activity Change to work
</commit_message>
<xml_diff>
--- a/Documentation/Design Analysis/ActivityChangeAnalysis.xlsx
+++ b/Documentation/Design Analysis/ActivityChangeAnalysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theod\Documents\Git\WeeklyReview\Documentation\Design Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9922838F-203E-4345-82F9-9A1F49C4EDA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2FA7B2-CB28-4668-9DD4-4164F9F78DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1830" windowWidth="29040" windowHeight="15720" xr2:uid="{AF8E6ADA-CA6D-4B2C-8717-C0E9AFA47492}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="21">
   <si>
     <t>Resulting DB</t>
   </si>
@@ -237,17 +237,16 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -788,45 +787,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A907353-0A12-4651-91E8-79FE5A0F68C7}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="7"/>
-      <c r="G2" s="6" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="6"/>
+      <c r="G2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="J2" s="2" t="s">
+      <c r="H2" s="6"/>
+      <c r="J2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="2"/>
+      <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -858,25 +857,32 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G4" s="4" t="s">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
         <v>10</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="J4" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="3" t="b">
+      <c r="K4" s="1" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
       <c r="J5" t="s">
         <v>9</v>
       </c>
@@ -885,36 +891,36 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="G8" s="2" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="G8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="J8" s="2" t="s">
+      <c r="H8" s="3"/>
+      <c r="J8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="2"/>
+      <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -955,19 +961,19 @@
       <c r="C10" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="3" t="b">
+      <c r="E10" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="J10" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="3" t="b">
+      <c r="K10" s="1" t="b">
         <v>1</v>
       </c>
     </row>
@@ -981,7 +987,7 @@
       <c r="C11" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="3" t="b">
+      <c r="E11" s="1" t="b">
         <v>1</v>
       </c>
       <c r="J11" t="s">
@@ -992,62 +998,62 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1">
         <v>10</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3" t="b">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1">
         <v>12</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3" t="b">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="G16" s="2" t="s">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="G16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H16" s="2"/>
-      <c r="J16" s="2" t="s">
+      <c r="H16" s="3"/>
+      <c r="J16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K16" s="2"/>
+      <c r="K16" s="3"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1091,34 +1097,34 @@
       <c r="D18" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="3" t="b">
+      <c r="E18" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="2" t="s">
         <v>20</v>
       </c>
       <c r="J18" t="s">
         <v>18</v>
       </c>
-      <c r="K18" s="3" t="b">
+      <c r="K18" s="1" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1">
         <v>16</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="3" t="b">
+      <c r="E19" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J19" t="s">
@@ -1129,11 +1135,6 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
       <c r="J20" t="s">
         <v>20</v>
       </c>
@@ -1141,15 +1142,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-    </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A1:K1"/>
     <mergeCell ref="A16:E16"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="J16:K16"/>
@@ -1158,10 +1156,6 @@
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="A15:K15"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="A1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="9">

</xml_diff>